<commit_message>
Updated Data base verification test cases
</commit_message>
<xml_diff>
--- a/OrangeHRMProject/src/test/resources/testdata/Test_data.xlsx
+++ b/OrangeHRMProject/src/test/resources/testdata/Test_data.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15756" windowHeight="4476"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15756" windowHeight="4476" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="validLoginTest" sheetId="1" r:id="rId1"/>
     <sheet name="invalidLoginTest" sheetId="2" r:id="rId2"/>
+    <sheet name="empDBVerification" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -32,7 +32,25 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>admin123</t>
+    <t>orangehrm_vani</t>
+  </si>
+  <si>
+    <t>Qweinav12!8</t>
+  </si>
+  <si>
+    <t>empID</t>
+  </si>
+  <si>
+    <t>empName</t>
+  </si>
+  <si>
+    <t>Vani Bhat</t>
+  </si>
+  <si>
+    <t>ashwin hebbar</t>
+  </si>
+  <si>
+    <t>sasha de della</t>
   </si>
 </sst>
 </file>
@@ -352,8 +370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -368,10 +386,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -408,4 +426,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>